<commit_message>
Update tek share methods
</commit_message>
<xml_diff>
--- a/input/TEK_ID.xlsx
+++ b/input/TEK_ID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\task_836\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ED0A60-C44C-4EC3-BC97-D0D2E5EF6F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B437D3-72DB-48E0-8C3C-8E2B269BE3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TEK_ID</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>TEK69_2</t>
+  </si>
+  <si>
+    <t>TEK69_3</t>
   </si>
 </sst>
 </file>
@@ -76,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +117,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -450,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B03D8-908D-4A3A-99BA-6E1BE1F7D81E}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,37 +495,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#1080 added SharesPerCondition, updated TEK class, Buildings and TEKParameters dataclass
</commit_message>
<xml_diff>
--- a/input/TEK_ID.xlsx
+++ b/input/TEK_ID.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\task_836\Energibruksmodell\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\work_space\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B437D3-72DB-48E0-8C3C-8E2B269BE3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549460A4-45C8-4DF3-B328-D0ACBAE44830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6075" yWindow="4050" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>TEK_ID</t>
-  </si>
-  <si>
     <t>TEK49</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>TEK69_3</t>
+  </si>
+  <si>
+    <t>TEK</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,62 +472,62 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated input data for TEK ID and Parameters, and added method to filter tek_list in Buildings
</commit_message>
<xml_diff>
--- a/input/TEK_ID.xlsx
+++ b/input/TEK_ID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\work_space\Energibruksmodell\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfep\work_space\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549460A4-45C8-4DF3-B328-D0ACBAE44830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BD93B4-EDEE-412E-B366-EBBD91194627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="4050" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>TEK49</t>
-  </si>
-  <si>
-    <t>TEK87</t>
-  </si>
-  <si>
-    <t>TEK97</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>TEK07</t>
   </si>
@@ -57,19 +48,43 @@
     <t>TEK21</t>
   </si>
   <si>
-    <t>PRE_TEK49</t>
-  </si>
-  <si>
-    <t>TEK69_1</t>
-  </si>
-  <si>
-    <t>TEK69_2</t>
-  </si>
-  <si>
-    <t>TEK69_3</t>
-  </si>
-  <si>
     <t>TEK</t>
+  </si>
+  <si>
+    <t>PRE_TEK49_RES1</t>
+  </si>
+  <si>
+    <t>PRE_TEK49_RES2</t>
+  </si>
+  <si>
+    <t>PRE_TEK49_COM</t>
+  </si>
+  <si>
+    <t>TEK49_RES</t>
+  </si>
+  <si>
+    <t>TEK49_COM</t>
+  </si>
+  <si>
+    <t>TEK69_RES1</t>
+  </si>
+  <si>
+    <t>TEK69_RES2</t>
+  </si>
+  <si>
+    <t>TEK69_COM</t>
+  </si>
+  <si>
+    <t>TEK87_RES</t>
+  </si>
+  <si>
+    <t>TEK87_COM</t>
+  </si>
+  <si>
+    <t>TEK97_RES</t>
+  </si>
+  <si>
+    <t>TEK97_COM</t>
   </si>
 </sst>
 </file>
@@ -154,8 +169,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -459,75 +473,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B03D8-908D-4A3A-99BA-6E1BE1F7D81E}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1088 small update to filter_tek_list method
</commit_message>
<xml_diff>
--- a/input/TEK_ID.xlsx
+++ b/input/TEK_ID.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfep\work_space\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BD93B4-EDEE-412E-B366-EBBD91194627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEC5E2E-1A27-464E-8358-999ECA9CBFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,12 +51,6 @@
     <t>TEK</t>
   </si>
   <si>
-    <t>PRE_TEK49_RES1</t>
-  </si>
-  <si>
-    <t>PRE_TEK49_RES2</t>
-  </si>
-  <si>
     <t>PRE_TEK49_COM</t>
   </si>
   <si>
@@ -66,12 +60,6 @@
     <t>TEK49_COM</t>
   </si>
   <si>
-    <t>TEK69_RES1</t>
-  </si>
-  <si>
-    <t>TEK69_RES2</t>
-  </si>
-  <si>
     <t>TEK69_COM</t>
   </si>
   <si>
@@ -85,6 +73,18 @@
   </si>
   <si>
     <t>TEK97_COM</t>
+  </si>
+  <si>
+    <t>PRE_TEK49_RES_1950</t>
+  </si>
+  <si>
+    <t>PRE_TEK49_RES_1940</t>
+  </si>
+  <si>
+    <t>TEK69_RES_1976</t>
+  </si>
+  <si>
+    <t>TEK69_RES_1986</t>
   </si>
 </sst>
 </file>
@@ -169,9 +169,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{BE8C0AF8-6F26-468C-BDCC-9B7D5669AE09}"/>
@@ -473,93 +474,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B03D8-908D-4A3A-99BA-6E1BE1F7D81E}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>

</xml_diff>